<commit_message>
try 1 rendu 1
</commit_message>
<xml_diff>
--- a/Airport_Data.xlsx
+++ b/Airport_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnauddebrito/Documents/Ecole/A5/Webscrapping/Web_scraping_Project_Flights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5943BA5C-B589-2140-BE80-23C352E74033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F07394-9144-CB4E-9C68-08E5BEA27C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{7949DA0D-536D-E149-ACCC-B2A1654D509C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="25">
   <si>
     <t>Departure_Airport</t>
   </si>
@@ -475,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E49B18-79BA-6348-BA83-75728AEE62F3}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,18 +519,18 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -546,11 +546,11 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -560,25 +560,25 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -589,24 +589,24 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,24 +617,24 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -645,10 +645,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,24 +659,24 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,18 +687,18 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -715,24 +715,24 @@
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -742,11 +742,11 @@
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -757,18 +757,18 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
@@ -784,11 +784,11 @@
       <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,25 +798,25 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>16</v>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,24 +827,24 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -855,24 +855,24 @@
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
+      <c r="A28" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -883,10 +883,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -897,24 +897,24 @@
         <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>16</v>
+      <c r="A31" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -925,18 +925,18 @@
         <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
@@ -953,32 +953,32 @@
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>22</v>
+      <c r="A35" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>16</v>
+      <c r="A36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
@@ -1009,18 +1009,18 @@
         <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>23</v>
+      <c r="A39" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>18</v>
@@ -1030,11 +1030,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>16</v>
+      <c r="A40" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>18</v>
@@ -1045,24 +1045,24 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>19</v>
@@ -1073,24 +1073,24 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>20</v>
@@ -1101,24 +1101,24 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>16</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>16</v>
@@ -1143,24 +1143,24 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>10</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>21</v>
@@ -1177,18 +1177,18 @@
         <v>12</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>22</v>
@@ -1198,25 +1198,25 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>23</v>
+      <c r="A52" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>16</v>
+      <c r="A53" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>17</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
@@ -1247,18 +1247,18 @@
         <v>14</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>23</v>
+      <c r="A56" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>18</v>
@@ -1268,11 +1268,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>16</v>
+      <c r="A57" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>18</v>
@@ -1283,24 +1283,24 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>19</v>
@@ -1311,24 +1311,24 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>20</v>
@@ -1339,24 +1339,24 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>16</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>16</v>
@@ -1381,71 +1381,29 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>10</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B68" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>